<commit_message>
Сделал orgApp_blocked.py, частично добавил в main_code.py open, closed, blocked
Есть "баги" - 1) появляется окно с кнопкой завершения работы ПК; 2) В случае приложений с большим кол-вом вкладок нужно проверка на условие с содержания значения, а не полное соответствие значению списка. Также, видимо, можно реализовать закрытие браузера, если открыта не та вкладка.

Далее: 1) Добавить Closed, open, blocked; 2) Записать в БД, что РБ не был выполнен, если кнопка Next не была нажата

Также обнаружил баг - Кнопка Hide в окне newWB скрывает правое-нижнее окно, а кнопка в
    правом-нижнем - окно newWB
</commit_message>
<xml_diff>
--- a/resources/settings/work_blocks.xlsx
+++ b/resources/settings/work_blocks.xlsx
@@ -300,7 +300,7 @@
     <t>Fun</t>
   </si>
   <si>
-    <t>Taskmgr.exe, mmc.exe, SystemSettings.exe | Пользователи, Локальный диск (C:), Свойства: abc, Разрешения для группы</t>
+    <t>Taskmgr.exe, mmc.exe, SystemSettings.exe | *, , Медиаплеер, Медиаплеер, , Калькулятор, Калькулятор, , , , , NVIDIA GeForce Overlay, Program Manager</t>
   </si>
   <si>
     <t>Work</t>
@@ -1332,7 +1332,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6:D7"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1379,7 +1379,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" s="2" customFormat="1" ht="28.8" spans="2:6">
+    <row r="4" s="2" customFormat="1" ht="43.2" spans="2:6">
       <c r="B4" s="10" t="s">
         <v>7</v>
       </c>

</xml_diff>